<commit_message>
update corona report excel
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-02-21.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-02-21.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="392">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -794,61 +794,61 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 23.2.</t>
+    <t xml:space="preserve">Stand 24.2.</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt-Bevölkerung</t>
   </si>
   <si>
-    <t xml:space="preserve">3413730 ( 4,1 %)</t>
+    <t xml:space="preserve">3518294 ( 4,2 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit nur 1 Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">1607124 ( 1,9 %)</t>
+    <t xml:space="preserve">1663366 ( 2,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit 2 Impfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">1806606 ( 2,2 %)</t>
+    <t xml:space="preserve">1854928 ( 2,2 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Pflegeheimbewohnende</t>
   </si>
   <si>
-    <t xml:space="preserve">772832 (97,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">244080 (30,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">528752 (66,5 %)</t>
+    <t xml:space="preserve">780493 (98,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240883 (30,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">539610 (67,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Über-80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">1446871 (25,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">788862 (13,9 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">658009 (11,6 %)</t>
+    <t xml:space="preserve">1503334 (26,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">825860 (14,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">677474 (11,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Personal in ...</t>
   </si>
   <si>
-    <t xml:space="preserve">1513677 (42,0 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">653886 (18,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">859791 (23,9 %)</t>
+    <t xml:space="preserve">1552902 (43,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">670495 (18,6 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">882407 (24,5 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt nur 1x</t>
@@ -875,270 +875,279 @@
     <t xml:space="preserve">7-Tage-Inzidenz 80+</t>
   </si>
   <si>
+    <t xml:space="preserve">2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,2</t>
+  </si>
+  <si>
     <t xml:space="preserve">1,9</t>
   </si>
   <si>
-    <t xml:space="preserve">2,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66,5</t>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71,8</t>
   </si>
   <si>
     <t xml:space="preserve">13,9</t>
   </si>
   <si>
-    <t xml:space="preserve">11,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,5</t>
+    <t xml:space="preserve"> 4,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,9</t>
   </si>
   <si>
     <t xml:space="preserve">78,5</t>
   </si>
   <si>
-    <t xml:space="preserve">16,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,5</t>
+    <t xml:space="preserve"> 7,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,4</t>
   </si>
   <si>
     <t xml:space="preserve">1,7</t>
   </si>
   <si>
-    <t xml:space="preserve">2,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82,7</t>
+    <t xml:space="preserve">35,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43,0</t>
   </si>
   <si>
     <t xml:space="preserve">14,1</t>
   </si>
   <si>
-    <t xml:space="preserve">2,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Impfstoffdosen</t>
   </si>
   <si>
@@ -1148,19 +1157,19 @@
     <t xml:space="preserve">Verabreichte Impfstoffdosen</t>
   </si>
   <si>
-    <t xml:space="preserve">5220336</t>
+    <t xml:space="preserve">5373222</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">3413730</t>
+    <t xml:space="preserve">3518294</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">1806606</t>
+    <t xml:space="preserve">1854928</t>
   </si>
   <si>
     <t xml:space="preserve">Nach Herstellern</t>
@@ -1169,34 +1178,34 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">4867212 ( 93,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3087374</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1779838</t>
+    <t xml:space="preserve">4987095 ( 92,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3160936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1826159</t>
   </si>
   <si>
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">141238 (  2,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26768</t>
+    <t xml:space="preserve">147571 (  2,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">118802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28769</t>
   </si>
   <si>
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">211886 (  4,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211886</t>
+    <t xml:space="preserve">238556 (  4,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">238556</t>
   </si>
 </sst>
 </file>
@@ -1727,25 +1736,25 @@
         <v>161</v>
       </c>
       <c r="B4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" t="s">
         <v>295</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>296</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>297</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>298</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>299</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>300</v>
-      </c>
-      <c r="H4" t="s">
-        <v>301</v>
       </c>
       <c r="I4" t="n">
         <v>57</v>
@@ -1759,25 +1768,25 @@
         <v>165</v>
       </c>
       <c r="B5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" t="s">
         <v>302</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>303</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>304</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>305</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>306</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>307</v>
-      </c>
-      <c r="H5" t="s">
-        <v>308</v>
       </c>
       <c r="I5" t="n">
         <v>55</v>
@@ -1791,25 +1800,25 @@
         <v>168</v>
       </c>
       <c r="B6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D6" t="s">
         <v>309</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>310</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>311</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>312</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>313</v>
-      </c>
-      <c r="G6" t="s">
-        <v>314</v>
-      </c>
-      <c r="H6" t="s">
-        <v>315</v>
       </c>
       <c r="I6" t="n">
         <v>63</v>
@@ -1823,25 +1832,25 @@
         <v>172</v>
       </c>
       <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" t="s">
         <v>316</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>317</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>318</v>
       </c>
-      <c r="E7" t="s">
-        <v>319</v>
-      </c>
-      <c r="F7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G7" t="s">
-        <v>228</v>
-      </c>
       <c r="H7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I7" t="n">
         <v>75</v>
@@ -1858,22 +1867,22 @@
         <v>289</v>
       </c>
       <c r="C8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" t="s">
         <v>321</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>322</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>323</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>324</v>
-      </c>
-      <c r="G8" t="s">
-        <v>325</v>
-      </c>
-      <c r="H8" t="s">
-        <v>326</v>
       </c>
       <c r="I8" t="n">
         <v>74</v>
@@ -1887,25 +1896,25 @@
         <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E9" t="s">
+        <v>326</v>
+      </c>
+      <c r="F9" t="s">
         <v>327</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>328</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>329</v>
-      </c>
-      <c r="G9" t="s">
-        <v>330</v>
-      </c>
-      <c r="H9" t="s">
-        <v>331</v>
       </c>
       <c r="I9" t="n">
         <v>61</v>
@@ -1919,25 +1928,25 @@
         <v>182</v>
       </c>
       <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D10" t="s">
+        <v>331</v>
+      </c>
+      <c r="E10" t="s">
         <v>332</v>
       </c>
-      <c r="C10" t="s">
-        <v>303</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>333</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>334</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>335</v>
-      </c>
-      <c r="G10" t="s">
-        <v>336</v>
-      </c>
-      <c r="H10" t="s">
-        <v>337</v>
       </c>
       <c r="I10" t="n">
         <v>64</v>
@@ -1954,22 +1963,22 @@
         <v>281</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
+        <v>336</v>
+      </c>
+      <c r="E11" t="s">
+        <v>337</v>
+      </c>
+      <c r="F11" t="s">
         <v>338</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>339</v>
       </c>
-      <c r="F11" t="s">
-        <v>340</v>
-      </c>
-      <c r="G11" t="s">
-        <v>341</v>
-      </c>
       <c r="H11" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
       <c r="I11" t="n">
         <v>62</v>
@@ -1983,22 +1992,22 @@
         <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C12" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="D12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" t="s">
         <v>342</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>343</v>
-      </c>
-      <c r="F12" t="s">
-        <v>344</v>
-      </c>
-      <c r="G12" t="s">
-        <v>345</v>
       </c>
       <c r="H12" t="s">
         <v>287</v>
@@ -2015,25 +2024,25 @@
         <v>192</v>
       </c>
       <c r="B13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D13" t="s">
         <v>346</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>347</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>348</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>349</v>
       </c>
-      <c r="F13" t="s">
-        <v>350</v>
-      </c>
-      <c r="G13" t="s">
-        <v>329</v>
-      </c>
       <c r="H13" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="I13" t="n">
         <v>52</v>
@@ -2047,10 +2056,10 @@
         <v>196</v>
       </c>
       <c r="B14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" t="s">
         <v>282</v>
-      </c>
-      <c r="C14" t="s">
-        <v>295</v>
       </c>
       <c r="D14" t="s">
         <v>351</v>
@@ -2065,7 +2074,7 @@
         <v>354</v>
       </c>
       <c r="H14" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="I14" t="n">
         <v>61</v>
@@ -2079,16 +2088,16 @@
         <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>350</v>
       </c>
       <c r="C15" t="s">
         <v>289</v>
       </c>
       <c r="D15" t="s">
+        <v>355</v>
+      </c>
+      <c r="E15" t="s">
         <v>356</v>
-      </c>
-      <c r="E15" t="s">
-        <v>338</v>
       </c>
       <c r="F15" t="s">
         <v>357</v>
@@ -2097,7 +2106,7 @@
         <v>358</v>
       </c>
       <c r="H15" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="I15" t="n">
         <v>68</v>
@@ -2111,22 +2120,22 @@
         <v>201</v>
       </c>
       <c r="B16" t="s">
-        <v>316</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
         <v>282</v>
       </c>
       <c r="D16" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E16" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F16" t="s">
-        <v>249</v>
+        <v>363</v>
       </c>
       <c r="G16" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="H16" t="s">
         <v>294</v>
@@ -2143,25 +2152,25 @@
         <v>204</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D17" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="E17" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="F17" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G17" t="s">
-        <v>299</v>
+        <v>368</v>
       </c>
       <c r="H17" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="I17" t="n">
         <v>50</v>
@@ -2175,25 +2184,25 @@
         <v>207</v>
       </c>
       <c r="B18" t="s">
-        <v>282</v>
+        <v>350</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D18" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E18" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F18" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
       <c r="G18" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="H18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I18" t="n">
         <v>119</v>
@@ -2218,15 +2227,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B2"/>
     </row>
@@ -2235,98 +2244,98 @@
         <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B7" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B8" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B9" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B11" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B13" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B14" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B15"/>
     </row>

</xml_diff>